<commit_message>
Atualizações dados 16/07 23h
</commit_message>
<xml_diff>
--- a/data/goal_match.xlsx
+++ b/data/goal_match.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +478,11 @@
           <t>scoreAway2nd</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>dt_insertion</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,6 +509,9 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -525,6 +537,9 @@
       </c>
       <c r="H3" t="n">
         <v>1</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45489</v>
       </c>
     </row>
     <row r="4">
@@ -552,6 +567,9 @@
       <c r="H4" t="n">
         <v>2</v>
       </c>
+      <c r="I4" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -578,6 +596,9 @@
       <c r="H5" t="n">
         <v>2</v>
       </c>
+      <c r="I5" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -604,6 +625,9 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
+      <c r="I6" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -630,6 +654,9 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -656,6 +683,9 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
+      <c r="I8" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -682,6 +712,9 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -708,6 +741,9 @@
       <c r="H10" t="n">
         <v>1</v>
       </c>
+      <c r="I10" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -734,6 +770,9 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
+      <c r="I11" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -760,6 +799,9 @@
       <c r="H12" t="n">
         <v>0</v>
       </c>
+      <c r="I12" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -786,6 +828,9 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
+      <c r="I13" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -812,6 +857,9 @@
       <c r="H14" t="n">
         <v>1</v>
       </c>
+      <c r="I14" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -838,6 +886,9 @@
       <c r="H15" t="n">
         <v>1</v>
       </c>
+      <c r="I15" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -864,6 +915,9 @@
       <c r="H16" t="n">
         <v>1</v>
       </c>
+      <c r="I16" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -890,6 +944,9 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
+      <c r="I17" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -916,6 +973,9 @@
       <c r="H18" t="n">
         <v>0</v>
       </c>
+      <c r="I18" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -942,6 +1002,9 @@
       <c r="H19" t="n">
         <v>1</v>
       </c>
+      <c r="I19" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -968,6 +1031,9 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
+      <c r="I20" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -994,6 +1060,9 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1020,6 +1089,9 @@
       <c r="H22" t="n">
         <v>1</v>
       </c>
+      <c r="I22" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1046,6 +1118,9 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1072,6 +1147,9 @@
       <c r="H24" t="n">
         <v>0</v>
       </c>
+      <c r="I24" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1098,6 +1176,9 @@
       <c r="H25" t="n">
         <v>0</v>
       </c>
+      <c r="I25" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1124,6 +1205,9 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1150,6 +1234,9 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1176,6 +1263,9 @@
       <c r="H28" t="n">
         <v>2</v>
       </c>
+      <c r="I28" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1202,6 +1292,9 @@
       <c r="H29" t="n">
         <v>2</v>
       </c>
+      <c r="I29" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1228,6 +1321,9 @@
       <c r="H30" t="n">
         <v>1</v>
       </c>
+      <c r="I30" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1254,6 +1350,9 @@
       <c r="H31" t="n">
         <v>3</v>
       </c>
+      <c r="I31" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1280,6 +1379,9 @@
       <c r="H32" t="n">
         <v>2</v>
       </c>
+      <c r="I32" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1306,6 +1408,9 @@
       <c r="H33" t="n">
         <v>0</v>
       </c>
+      <c r="I33" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1332,6 +1437,9 @@
       <c r="H34" t="n">
         <v>2</v>
       </c>
+      <c r="I34" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1358,6 +1466,9 @@
       <c r="H35" t="n">
         <v>0</v>
       </c>
+      <c r="I35" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1384,6 +1495,9 @@
       <c r="H36" t="n">
         <v>1</v>
       </c>
+      <c r="I36" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1410,6 +1524,9 @@
       <c r="H37" t="n">
         <v>0</v>
       </c>
+      <c r="I37" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1436,6 +1553,9 @@
       <c r="H38" t="n">
         <v>1</v>
       </c>
+      <c r="I38" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1462,6 +1582,9 @@
       <c r="H39" t="n">
         <v>1</v>
       </c>
+      <c r="I39" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1488,6 +1611,9 @@
       <c r="H40" t="n">
         <v>0</v>
       </c>
+      <c r="I40" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1514,6 +1640,9 @@
       <c r="H41" t="n">
         <v>2</v>
       </c>
+      <c r="I41" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1540,6 +1669,9 @@
       <c r="H42" t="n">
         <v>1</v>
       </c>
+      <c r="I42" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1566,6 +1698,9 @@
       <c r="H43" t="n">
         <v>0</v>
       </c>
+      <c r="I43" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1592,6 +1727,9 @@
       <c r="H44" t="n">
         <v>0</v>
       </c>
+      <c r="I44" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1618,6 +1756,9 @@
       <c r="H45" t="n">
         <v>2</v>
       </c>
+      <c r="I45" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1644,6 +1785,9 @@
       <c r="H46" t="n">
         <v>1</v>
       </c>
+      <c r="I46" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1670,6 +1814,9 @@
       <c r="H47" t="n">
         <v>1</v>
       </c>
+      <c r="I47" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1696,6 +1843,9 @@
       <c r="H48" t="n">
         <v>0</v>
       </c>
+      <c r="I48" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1722,6 +1872,9 @@
       <c r="H49" t="n">
         <v>0</v>
       </c>
+      <c r="I49" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1748,6 +1901,9 @@
       <c r="H50" t="n">
         <v>1</v>
       </c>
+      <c r="I50" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1774,6 +1930,9 @@
       <c r="H51" t="n">
         <v>0</v>
       </c>
+      <c r="I51" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1800,6 +1959,9 @@
       <c r="H52" t="n">
         <v>1</v>
       </c>
+      <c r="I52" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1826,6 +1988,9 @@
       <c r="H53" t="n">
         <v>0</v>
       </c>
+      <c r="I53" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1852,6 +2017,9 @@
       <c r="H54" t="n">
         <v>1</v>
       </c>
+      <c r="I54" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1878,6 +2046,9 @@
       <c r="H55" t="n">
         <v>0</v>
       </c>
+      <c r="I55" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1904,6 +2075,9 @@
       <c r="H56" t="n">
         <v>2</v>
       </c>
+      <c r="I56" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1930,6 +2104,9 @@
       <c r="H57" t="n">
         <v>1</v>
       </c>
+      <c r="I57" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1956,6 +2133,9 @@
       <c r="H58" t="n">
         <v>1</v>
       </c>
+      <c r="I58" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1982,6 +2162,9 @@
       <c r="H59" t="n">
         <v>1</v>
       </c>
+      <c r="I59" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2008,6 +2191,9 @@
       <c r="H60" t="n">
         <v>1</v>
       </c>
+      <c r="I60" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2034,6 +2220,9 @@
       <c r="H61" t="n">
         <v>1</v>
       </c>
+      <c r="I61" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2060,6 +2249,9 @@
       <c r="H62" t="n">
         <v>1</v>
       </c>
+      <c r="I62" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2086,6 +2278,9 @@
       <c r="H63" t="n">
         <v>2</v>
       </c>
+      <c r="I63" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2112,6 +2307,9 @@
       <c r="H64" t="n">
         <v>3</v>
       </c>
+      <c r="I64" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2138,6 +2336,9 @@
       <c r="H65" t="n">
         <v>0</v>
       </c>
+      <c r="I65" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2164,6 +2365,9 @@
       <c r="H66" t="n">
         <v>0</v>
       </c>
+      <c r="I66" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2190,6 +2394,9 @@
       <c r="H67" t="n">
         <v>1</v>
       </c>
+      <c r="I67" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2216,6 +2423,9 @@
       <c r="H68" t="n">
         <v>0</v>
       </c>
+      <c r="I68" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2242,6 +2452,9 @@
       <c r="H69" t="n">
         <v>0</v>
       </c>
+      <c r="I69" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2268,6 +2481,9 @@
       <c r="H70" t="n">
         <v>0</v>
       </c>
+      <c r="I70" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2294,6 +2510,9 @@
       <c r="H71" t="n">
         <v>1</v>
       </c>
+      <c r="I71" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2320,6 +2539,9 @@
       <c r="H72" t="n">
         <v>0</v>
       </c>
+      <c r="I72" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2346,6 +2568,9 @@
       <c r="H73" t="n">
         <v>1</v>
       </c>
+      <c r="I73" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2372,6 +2597,9 @@
       <c r="H74" t="n">
         <v>0</v>
       </c>
+      <c r="I74" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2398,6 +2626,9 @@
       <c r="H75" t="n">
         <v>0</v>
       </c>
+      <c r="I75" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -2424,6 +2655,9 @@
       <c r="H76" t="n">
         <v>0</v>
       </c>
+      <c r="I76" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2450,6 +2684,9 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -2476,6 +2713,9 @@
       <c r="H78" t="n">
         <v>2</v>
       </c>
+      <c r="I78" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2502,6 +2742,9 @@
       <c r="H79" t="n">
         <v>1</v>
       </c>
+      <c r="I79" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2528,6 +2771,9 @@
       <c r="H80" t="n">
         <v>0</v>
       </c>
+      <c r="I80" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2554,6 +2800,9 @@
       <c r="H81" t="n">
         <v>1</v>
       </c>
+      <c r="I81" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -2580,6 +2829,9 @@
       <c r="H82" t="n">
         <v>2</v>
       </c>
+      <c r="I82" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -2606,6 +2858,9 @@
       <c r="H83" t="n">
         <v>0</v>
       </c>
+      <c r="I83" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -2632,6 +2887,9 @@
       <c r="H84" t="n">
         <v>1</v>
       </c>
+      <c r="I84" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -2658,6 +2916,9 @@
       <c r="H85" t="n">
         <v>0</v>
       </c>
+      <c r="I85" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -2684,6 +2945,9 @@
       <c r="H86" t="n">
         <v>3</v>
       </c>
+      <c r="I86" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -2710,6 +2974,9 @@
       <c r="H87" t="n">
         <v>2</v>
       </c>
+      <c r="I87" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -2736,6 +3003,9 @@
       <c r="H88" t="n">
         <v>1</v>
       </c>
+      <c r="I88" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2762,6 +3032,9 @@
       <c r="H89" t="n">
         <v>0</v>
       </c>
+      <c r="I89" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -2788,6 +3061,9 @@
       <c r="H90" t="n">
         <v>0</v>
       </c>
+      <c r="I90" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -2814,6 +3090,9 @@
       <c r="H91" t="n">
         <v>1</v>
       </c>
+      <c r="I91" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2840,6 +3119,9 @@
       <c r="H92" t="n">
         <v>0</v>
       </c>
+      <c r="I92" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2866,6 +3148,9 @@
       <c r="H93" t="n">
         <v>0</v>
       </c>
+      <c r="I93" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2892,6 +3177,9 @@
       <c r="H94" t="n">
         <v>1</v>
       </c>
+      <c r="I94" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2918,6 +3206,9 @@
       <c r="H95" t="n">
         <v>0</v>
       </c>
+      <c r="I95" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2944,6 +3235,9 @@
       <c r="H96" t="n">
         <v>1</v>
       </c>
+      <c r="I96" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2970,6 +3264,9 @@
       <c r="H97" t="n">
         <v>1</v>
       </c>
+      <c r="I97" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2996,6 +3293,9 @@
       <c r="H98" t="n">
         <v>1</v>
       </c>
+      <c r="I98" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -3022,6 +3322,9 @@
       <c r="H99" t="n">
         <v>0</v>
       </c>
+      <c r="I99" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -3048,6 +3351,9 @@
       <c r="H100" t="n">
         <v>0</v>
       </c>
+      <c r="I100" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -3074,6 +3380,9 @@
       <c r="H101" t="n">
         <v>1</v>
       </c>
+      <c r="I101" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -3100,6 +3409,9 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -3126,6 +3438,9 @@
       <c r="H103" t="n">
         <v>1</v>
       </c>
+      <c r="I103" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -3152,6 +3467,9 @@
       <c r="H104" t="n">
         <v>0</v>
       </c>
+      <c r="I104" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -3178,6 +3496,9 @@
       <c r="H105" t="n">
         <v>1</v>
       </c>
+      <c r="I105" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -3204,6 +3525,9 @@
       <c r="H106" t="n">
         <v>0</v>
       </c>
+      <c r="I106" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -3230,6 +3554,9 @@
       <c r="H107" t="n">
         <v>0</v>
       </c>
+      <c r="I107" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -3256,6 +3583,9 @@
       <c r="H108" t="n">
         <v>0</v>
       </c>
+      <c r="I108" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -3282,6 +3612,9 @@
       <c r="H109" t="n">
         <v>1</v>
       </c>
+      <c r="I109" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -3308,6 +3641,9 @@
       <c r="H110" t="n">
         <v>0</v>
       </c>
+      <c r="I110" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -3334,6 +3670,9 @@
       <c r="H111" t="n">
         <v>0</v>
       </c>
+      <c r="I111" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -3360,6 +3699,9 @@
       <c r="H112" t="n">
         <v>0</v>
       </c>
+      <c r="I112" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -3386,6 +3728,9 @@
       <c r="H113" t="n">
         <v>0</v>
       </c>
+      <c r="I113" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -3412,6 +3757,9 @@
       <c r="H114" t="n">
         <v>2</v>
       </c>
+      <c r="I114" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -3438,6 +3786,9 @@
       <c r="H115" t="n">
         <v>1</v>
       </c>
+      <c r="I115" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -3464,6 +3815,9 @@
       <c r="H116" t="n">
         <v>1</v>
       </c>
+      <c r="I116" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -3490,6 +3844,9 @@
       <c r="H117" t="n">
         <v>0</v>
       </c>
+      <c r="I117" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -3516,6 +3873,9 @@
       <c r="H118" t="n">
         <v>1</v>
       </c>
+      <c r="I118" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -3542,6 +3902,9 @@
       <c r="H119" t="n">
         <v>0</v>
       </c>
+      <c r="I119" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -3568,6 +3931,9 @@
       <c r="H120" t="n">
         <v>1</v>
       </c>
+      <c r="I120" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -3594,6 +3960,9 @@
       <c r="H121" t="n">
         <v>0</v>
       </c>
+      <c r="I121" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -3620,6 +3989,9 @@
       <c r="H122" t="n">
         <v>1</v>
       </c>
+      <c r="I122" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -3646,6 +4018,9 @@
       <c r="H123" t="n">
         <v>0</v>
       </c>
+      <c r="I123" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -3672,6 +4047,9 @@
       <c r="H124" t="n">
         <v>0</v>
       </c>
+      <c r="I124" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -3698,6 +4076,9 @@
       <c r="H125" t="n">
         <v>1</v>
       </c>
+      <c r="I125" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -3724,6 +4105,9 @@
       <c r="H126" t="n">
         <v>0</v>
       </c>
+      <c r="I126" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -3750,6 +4134,9 @@
       <c r="H127" t="n">
         <v>1</v>
       </c>
+      <c r="I127" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -3776,6 +4163,9 @@
       <c r="H128" t="n">
         <v>0</v>
       </c>
+      <c r="I128" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -3802,6 +4192,9 @@
       <c r="H129" t="n">
         <v>0</v>
       </c>
+      <c r="I129" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -3828,6 +4221,9 @@
       <c r="H130" t="n">
         <v>1</v>
       </c>
+      <c r="I130" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -3854,6 +4250,9 @@
       <c r="H131" t="n">
         <v>2</v>
       </c>
+      <c r="I131" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -3880,6 +4279,9 @@
       <c r="H132" t="n">
         <v>0</v>
       </c>
+      <c r="I132" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -3906,6 +4308,9 @@
       <c r="H133" t="n">
         <v>0</v>
       </c>
+      <c r="I133" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -3932,6 +4337,9 @@
       <c r="H134" t="n">
         <v>2</v>
       </c>
+      <c r="I134" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -3958,6 +4366,9 @@
       <c r="H135" t="n">
         <v>1</v>
       </c>
+      <c r="I135" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -3984,6 +4395,9 @@
       <c r="H136" t="n">
         <v>0</v>
       </c>
+      <c r="I136" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -4010,6 +4424,9 @@
       <c r="H137" t="n">
         <v>0</v>
       </c>
+      <c r="I137" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -4036,6 +4453,9 @@
       <c r="H138" t="n">
         <v>0</v>
       </c>
+      <c r="I138" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -4062,6 +4482,9 @@
       <c r="H139" t="n">
         <v>0</v>
       </c>
+      <c r="I139" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -4088,6 +4511,9 @@
       <c r="H140" t="n">
         <v>0</v>
       </c>
+      <c r="I140" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -4114,6 +4540,9 @@
       <c r="H141" t="n">
         <v>0</v>
       </c>
+      <c r="I141" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -4140,6 +4569,9 @@
       <c r="H142" t="n">
         <v>2</v>
       </c>
+      <c r="I142" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -4166,6 +4598,9 @@
       <c r="H143" t="n">
         <v>2</v>
       </c>
+      <c r="I143" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4192,6 +4627,9 @@
       <c r="H144" t="n">
         <v>0</v>
       </c>
+      <c r="I144" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -4218,6 +4656,9 @@
       <c r="H145" t="n">
         <v>0</v>
       </c>
+      <c r="I145" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -4244,6 +4685,9 @@
       <c r="H146" t="n">
         <v>0</v>
       </c>
+      <c r="I146" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -4270,6 +4714,9 @@
       <c r="H147" t="n">
         <v>0</v>
       </c>
+      <c r="I147" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -4296,6 +4743,9 @@
       <c r="H148" t="n">
         <v>1</v>
       </c>
+      <c r="I148" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -4322,6 +4772,9 @@
       <c r="H149" t="n">
         <v>0</v>
       </c>
+      <c r="I149" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -4348,6 +4801,9 @@
       <c r="H150" t="n">
         <v>0</v>
       </c>
+      <c r="I150" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -4374,6 +4830,9 @@
       <c r="H151" t="n">
         <v>1</v>
       </c>
+      <c r="I151" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -4400,6 +4859,9 @@
       <c r="H152" t="n">
         <v>1</v>
       </c>
+      <c r="I152" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -4426,6 +4888,9 @@
       <c r="H153" t="n">
         <v>0</v>
       </c>
+      <c r="I153" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -4452,6 +4917,9 @@
       <c r="H154" t="n">
         <v>1</v>
       </c>
+      <c r="I154" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -4478,6 +4946,9 @@
       <c r="H155" t="n">
         <v>1</v>
       </c>
+      <c r="I155" s="2" t="n">
+        <v>45489</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -4503,6 +4974,67 @@
       </c>
       <c r="H156" t="n">
         <v>1</v>
+      </c>
+      <c r="I156" s="2" t="n">
+        <v>45489</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="n">
+        <v>12117143</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="n">
+        <v>1</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" s="2" t="n">
+        <v>45489.96614583334</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="n">
+        <v>12117139</v>
+      </c>
+      <c r="C158" t="n">
+        <v>2</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1</v>
+      </c>
+      <c r="G158" t="n">
+        <v>2</v>
+      </c>
+      <c r="H158" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" s="2" t="n">
+        <v>45489.96614583334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizações dados 17/07 00h
</commit_message>
<xml_diff>
--- a/data/goal_match.xlsx
+++ b/data/goal_match.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5037,6 +5037,35 @@
         <v>45489.96614583334</v>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="n">
+        <v>12117139</v>
+      </c>
+      <c r="C159" t="n">
+        <v>2</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0</v>
+      </c>
+      <c r="F159" t="n">
+        <v>1</v>
+      </c>
+      <c r="G159" t="n">
+        <v>2</v>
+      </c>
+      <c r="H159" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" s="2" t="n">
+        <v>45490.00260416666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizações dados 18/07 00h
</commit_message>
<xml_diff>
--- a/data/goal_match.xlsx
+++ b/data/goal_match.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5066,6 +5066,122 @@
         <v>45490.00260416666</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="n">
+        <v>12117142</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" t="n">
+        <v>1</v>
+      </c>
+      <c r="I160" s="2" t="n">
+        <v>45491.00302083333</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="n">
+        <v>12117140</v>
+      </c>
+      <c r="C161" t="n">
+        <v>1</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" s="2" t="n">
+        <v>45491.00302083333</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="n">
+        <v>12117138</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" t="n">
+        <v>0</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>1</v>
+      </c>
+      <c r="H162" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" s="2" t="n">
+        <v>45491.00302083333</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="n">
+        <v>12117141</v>
+      </c>
+      <c r="C163" t="n">
+        <v>3</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" t="n">
+        <v>2</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>1</v>
+      </c>
+      <c r="H163" t="n">
+        <v>1</v>
+      </c>
+      <c r="I163" s="2" t="n">
+        <v>45491.00302083333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizações dados 19/07 16h
</commit_message>
<xml_diff>
--- a/data/goal_match.xlsx
+++ b/data/goal_match.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="3">
@@ -539,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="4">
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="6">
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="7">
@@ -655,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="8">
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="9">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="10">
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="11">
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="12">
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="14">
@@ -858,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="15">
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="16">
@@ -916,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="17">
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="18">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="19">
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="20">
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="21">
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="22">
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="23">
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="24">
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="25">
@@ -1177,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="26">
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="27">
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="28">
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="29">
@@ -1293,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="30">
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="31">
@@ -1351,7 +1351,7 @@
         <v>3</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="32">
@@ -1380,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="33">
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="34">
@@ -1438,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="35">
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="36">
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="37">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="38">
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="39">
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="40">
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="41">
@@ -1641,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="42">
@@ -1670,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="43">
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="44">
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="45">
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="46">
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="47">
@@ -1815,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="48">
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="49">
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="50">
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="51">
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="52">
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="53">
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="54">
@@ -2018,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="55">
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="56">
@@ -2076,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="57">
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="58">
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="59">
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="60">
@@ -2192,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="61">
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="62">
@@ -2250,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="63">
@@ -2279,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="64">
@@ -2308,7 +2308,7 @@
         <v>3</v>
       </c>
       <c r="I64" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="65">
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="66">
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="67">
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="68">
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="69">
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="70">
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="71">
@@ -2511,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="72">
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="73">
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="74">
@@ -2598,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="75">
@@ -2627,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="76">
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="77">
@@ -2685,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="78">
@@ -2714,7 +2714,7 @@
         <v>2</v>
       </c>
       <c r="I78" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="79">
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="80">
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="81">
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="82">
@@ -2830,7 +2830,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="83">
@@ -2859,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="84">
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="I84" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="85">
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="86">
@@ -2946,7 +2946,7 @@
         <v>3</v>
       </c>
       <c r="I86" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="87">
@@ -2975,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="I87" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="88">
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="I88" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="89">
@@ -3033,7 +3033,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="90">
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="91">
@@ -3091,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="I91" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="92">
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="I92" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="93">
@@ -3149,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="94">
@@ -3178,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="I94" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="95">
@@ -3207,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="I95" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="96">
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="I96" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="97">
@@ -3265,7 +3265,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="98">
@@ -3294,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="I98" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="99">
@@ -3323,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="I99" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="100">
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="I100" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="101">
@@ -3381,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="I101" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="102">
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="I102" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="103">
@@ -3439,7 +3439,7 @@
         <v>1</v>
       </c>
       <c r="I103" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="104">
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="I104" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="105">
@@ -3497,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="I105" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="106">
@@ -3526,7 +3526,7 @@
         <v>0</v>
       </c>
       <c r="I106" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="107">
@@ -3555,7 +3555,7 @@
         <v>0</v>
       </c>
       <c r="I107" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="108">
@@ -3584,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="I108" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="109">
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="I109" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="110">
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="I110" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="111">
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="I111" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="112">
@@ -3700,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="I112" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="113">
@@ -3729,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="I113" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="114">
@@ -3758,7 +3758,7 @@
         <v>2</v>
       </c>
       <c r="I114" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="115">
@@ -3787,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="I115" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="116">
@@ -3816,7 +3816,7 @@
         <v>1</v>
       </c>
       <c r="I116" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="117">
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="I117" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="118">
@@ -3874,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="I118" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="119">
@@ -3903,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="I119" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="120">
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="I120" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="121">
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="I121" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="122">
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="I122" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="123">
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="I123" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="124">
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="I124" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="125">
@@ -4077,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="I125" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="126">
@@ -4106,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="I126" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="127">
@@ -4135,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="I127" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="128">
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="I128" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="129">
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="I129" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="130">
@@ -4222,7 +4222,7 @@
         <v>1</v>
       </c>
       <c r="I130" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="131">
@@ -4251,7 +4251,7 @@
         <v>2</v>
       </c>
       <c r="I131" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="132">
@@ -4280,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="I132" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="133">
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="I133" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="134">
@@ -4338,7 +4338,7 @@
         <v>2</v>
       </c>
       <c r="I134" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="135">
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="I135" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="136">
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="I136" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="137">
@@ -4425,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="I137" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="138">
@@ -4454,7 +4454,7 @@
         <v>0</v>
       </c>
       <c r="I138" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="139">
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
       <c r="I139" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="140">
@@ -4512,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="I140" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="141">
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="I141" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="142">
@@ -4570,7 +4570,7 @@
         <v>2</v>
       </c>
       <c r="I142" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="143">
@@ -4599,7 +4599,7 @@
         <v>2</v>
       </c>
       <c r="I143" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="144">
@@ -4628,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="I144" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="145">
@@ -4657,7 +4657,7 @@
         <v>0</v>
       </c>
       <c r="I145" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="146">
@@ -4686,7 +4686,7 @@
         <v>0</v>
       </c>
       <c r="I146" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="147">
@@ -4715,7 +4715,7 @@
         <v>0</v>
       </c>
       <c r="I147" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="148">
@@ -4744,7 +4744,7 @@
         <v>1</v>
       </c>
       <c r="I148" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="149">
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="I149" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="150">
@@ -4802,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="I150" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="151">
@@ -4831,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="I151" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="152">
@@ -4860,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="I152" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="153">
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="I153" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="154">
@@ -4918,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="I154" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="155">
@@ -4947,7 +4947,7 @@
         <v>1</v>
       </c>
       <c r="I155" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="156">
@@ -4976,7 +4976,7 @@
         <v>1</v>
       </c>
       <c r="I156" s="2" t="n">
-        <v>45489</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="157">
@@ -5005,7 +5005,7 @@
         <v>0</v>
       </c>
       <c r="I157" s="2" t="n">
-        <v>45489.96614583334</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="158">
@@ -5034,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="I158" s="2" t="n">
-        <v>45489.96614583334</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="159">
@@ -5042,10 +5042,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="n">
-        <v>12117139</v>
+        <v>12117142</v>
       </c>
       <c r="C159" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D159" t="n">
         <v>1</v>
@@ -5054,16 +5054,16 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G159" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I159" s="2" t="n">
-        <v>45490.00260416666</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="160">
@@ -5071,16 +5071,16 @@
         <v>159</v>
       </c>
       <c r="B160" t="n">
-        <v>12117142</v>
+        <v>12117140</v>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
@@ -5089,10 +5089,10 @@
         <v>0</v>
       </c>
       <c r="H160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I160" s="2" t="n">
-        <v>45491.00302083333</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="161">
@@ -5100,7 +5100,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="n">
-        <v>12117140</v>
+        <v>12117138</v>
       </c>
       <c r="C161" t="n">
         <v>1</v>
@@ -5109,19 +5109,19 @@
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F161" t="n">
         <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161" t="n">
         <v>0</v>
       </c>
       <c r="I161" s="2" t="n">
-        <v>45491.00302083333</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
     <row r="162">
@@ -5129,16 +5129,16 @@
         <v>161</v>
       </c>
       <c r="B162" t="n">
-        <v>12117138</v>
+        <v>12117141</v>
       </c>
       <c r="C162" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F162" t="n">
         <v>0</v>
@@ -5147,39 +5147,10 @@
         <v>1</v>
       </c>
       <c r="H162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I162" s="2" t="n">
-        <v>45491.00302083333</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>162</v>
-      </c>
-      <c r="B163" t="n">
-        <v>12117141</v>
-      </c>
-      <c r="C163" t="n">
-        <v>3</v>
-      </c>
-      <c r="D163" t="n">
-        <v>1</v>
-      </c>
-      <c r="E163" t="n">
-        <v>2</v>
-      </c>
-      <c r="F163" t="n">
-        <v>0</v>
-      </c>
-      <c r="G163" t="n">
-        <v>1</v>
-      </c>
-      <c r="H163" t="n">
-        <v>1</v>
-      </c>
-      <c r="I163" s="2" t="n">
-        <v>45491.00302083333</v>
+        <v>45492.6733912037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>